<commit_message>
Permitindo outros uploads das outras planilhas
</commit_message>
<xml_diff>
--- a/dados/contador.xlsx
+++ b/dados/contador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\2DSTB-12\Disciplinas\PWBE\Integrador\Dados Integrador\Dados Integrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49374446898\Documents\SmartCity_Backend\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B5313-96AE-448E-9C78-143AC1425F69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FE3760-CCE4-4C87-990C-CA003C72900A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,17 +58,17 @@
     <t>uni</t>
   </si>
   <si>
-    <t>true</t>
+    <t>ativo</t>
   </si>
   <si>
-    <t>false</t>
+    <t>inativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +78,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,11 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:M201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +487,7 @@
     <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -518,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -538,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -558,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -578,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -598,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -618,7 +627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -638,7 +647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -658,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -678,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -698,7 +707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -718,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -738,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -758,7 +767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -778,7 +787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -797,6 +806,7 @@
       <c r="F16" t="s">
         <v>12</v>
       </c>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4500,5 +4510,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>